<commit_message>
Added Priority Queue with custom Comparator
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe9eed952d0f987d/Desktop/Interview-Preparation-Materials/Java-DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65DB1C14-A191-4238-BC48-3ED1B8427B83}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D26EE45-FB72-417E-BFD4-34BDDB79F5BF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1728,6 +1728,10 @@
 </file>
 
 <file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2030,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -3478,7 +3482,7 @@
       <c r="A140" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B140" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C140" s="4" t="s">

</xml_diff>

<commit_message>
Shortest Unique Prefix - Trie
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe9eed952d0f987d/Desktop/Interview-Preparation-Materials/Java-DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D26EE45-FB72-417E-BFD4-34BDDB79F5BF}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{340B6696-7EDB-4569-913A-B76E2DDCFAE8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1570,7 +1570,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1619,6 +1619,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1633,7 +1639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1677,6 +1683,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1732,6 +1739,10 @@
 </file>
 
 <file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person9.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2034,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
+      <selection activeCell="B402" sqref="B402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -6250,7 +6261,7 @@
       <c r="A402" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="B402" s="6" t="s">
+      <c r="B402" s="29" t="s">
         <v>383</v>
       </c>
       <c r="C402" s="4" t="s">

</xml_diff>

<commit_message>
Added Print all anagrams together
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe9eed952d0f987d/Desktop/Interview-Preparation-Materials/Java-DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A900784C-0B3E-4447-92AA-D816135DEC64}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{917FDCB6-1156-4C54-9421-B81CA64C2E86}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1715,6 +1715,10 @@
 </file>
 
 <file path=xl/persons/person10.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person11.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2049,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
-      <selection activeCell="A336" sqref="A336"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="B405" sqref="B405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -6298,7 +6302,7 @@
       <c r="A405" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="B405" s="6" t="s">
+      <c r="B405" s="29" t="s">
         <v>86</v>
       </c>
       <c r="C405" s="4" t="s">

</xml_diff>

<commit_message>
Added Heap & trie
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe9eed952d0f987d/Desktop/Interview-Preparation-Materials/Java-DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{917FDCB6-1156-4C54-9421-B81CA64C2E86}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{C6494043-9AED-46B9-A64C-EBC1E8A3D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D519250-201D-4DA9-BD0D-ADC1C382C5D5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1719,6 +1719,10 @@
 </file>
 
 <file path=xl/persons/person11.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person12.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2053,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
-      <selection activeCell="B405" sqref="B405"/>
+    <sheetView tabSelected="1" topLeftCell="C398" workbookViewId="0">
+      <selection activeCell="C403" sqref="C403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -6283,7 +6287,7 @@
       <c r="B403" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="C403" s="4" t="s">
+      <c r="C403" s="27" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6324,7 +6328,7 @@
       <c r="A407" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="B407" s="6" t="s">
+      <c r="B407" s="29" t="s">
         <v>387</v>
       </c>
       <c r="C407" s="4" t="s">

</xml_diff>